<commit_message>
[Distiller] More docs about distillation.
</commit_message>
<xml_diff>
--- a/distiller/doc/odbior_przedgonow_tylko_wg_termometrow_lesgo58.xlsx
+++ b/distiller/doc/odbior_przedgonow_tylko_wg_termometrow_lesgo58.xlsx
@@ -71,7 +71,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Moja inwencja: temperatura głowicy zaokrąglona do 0,1 stopnia Celsjusza, co ma na celu zasymulowanie termometru o mniejszej dokładności i rozdzielczości. 
-Pomysł jest taki by obserwować asymptotyczne dążenie do pewnej temperatury. Jeżeli temperatura już nie będzie dalej wzrastać to można podjąć decyzję o odbiorze serca. Trzeba porównać jak się ma ta decyzja do decyzji odbioru serca przy termometrze o dokładności 0,01. Prawdopodobnie termometr o mniejszej dokładności podejmie decyzję szybciej niz termometr o większej dokładności.
+Pomysł jest taki by obserwować asymptotyczne dążenie do pewnej temperatury. Jeżeli temperatura już nie będzie dalej wzrastać to można podjąć decyzję o odbiorze serca. Trzeba porównać jak się ma ta decyzja do decyzji odbioru serca przy termometrze o dokładności 0,01. Prawdopodobnie termometr o mniejszej dokładności podejmie decyzję szybciej niż termometr o większej dokładności.
 </t>
         </r>
       </text>
@@ -132,7 +132,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Przez 5min tem pozostaje 78,3125</t>
+          <t>Przez 5min tem pozostaje 78,25</t>
         </r>
       </text>
     </comment>
@@ -1181,6 +1181,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="599767424"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2100,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2342,7 +2343,7 @@
         <v>77.900000000000006</v>
       </c>
       <c r="E13">
-        <f>($D13-$D12)/($B13-$B12)</f>
+        <f t="shared" ref="E13:E31" si="2">($D13-$D12)/($B13-$B12)</f>
         <v>2.6666666666670835E-2</v>
       </c>
       <c r="F13">
@@ -2357,7 +2358,7 @@
         <v>77.875</v>
       </c>
       <c r="K13">
-        <f>($J13-$J12)/($B13-$B12)</f>
+        <f t="shared" ref="K13:K31" si="3">($J13-$J12)/($B13-$B12)</f>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="M13">
@@ -2365,7 +2366,7 @@
         <v>77.900000000000006</v>
       </c>
       <c r="N13">
-        <f>($M13-$M12)/($B13-$B12)</f>
+        <f t="shared" ref="N13:N31" si="4">($M13-$M12)/($B13-$B12)</f>
         <v>3.3333333333331439E-2</v>
       </c>
     </row>
@@ -2383,11 +2384,11 @@
         <v>77.95</v>
       </c>
       <c r="E14">
-        <f>($D14-$D13)/($B14-$B13)</f>
+        <f t="shared" si="2"/>
         <v>1.6666666666665719E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F31" si="2">ROUNDDOWN(E14/0.001 + 0.51,0) * 0.001</f>
+        <f t="shared" ref="F14:F31" si="5">ROUNDDOWN(E14/0.001 + 0.51,0) * 0.001</f>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="G14" s="4">
@@ -2398,7 +2399,7 @@
         <v>77.9375</v>
       </c>
       <c r="K14">
-        <f>($J14-$J13)/($B14-$B13)</f>
+        <f t="shared" si="3"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="M14">
@@ -2406,7 +2407,7 @@
         <v>78</v>
       </c>
       <c r="N14">
-        <f>($M14-$M13)/($B14-$B13)</f>
+        <f t="shared" si="4"/>
         <v>3.3333333333331439E-2</v>
       </c>
     </row>
@@ -2424,11 +2425,11 @@
         <v>77.989999999999995</v>
       </c>
       <c r="E15">
-        <f>($D15-$D14)/($B15-$B14)</f>
+        <f t="shared" si="2"/>
         <v>1.9999999999996021E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="G15" s="4">
@@ -2439,7 +2440,7 @@
         <v>78</v>
       </c>
       <c r="K15">
-        <f>($J15-$J14)/($B15-$B14)</f>
+        <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
       <c r="M15">
@@ -2447,7 +2448,7 @@
         <v>78</v>
       </c>
       <c r="N15">
-        <f>($M15-$M14)/($B15-$B14)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2465,11 +2466,11 @@
         <v>78.02</v>
       </c>
       <c r="E16">
-        <f>($D16-$D15)/($B16-$B15)</f>
+        <f t="shared" si="2"/>
         <v>1.5000000000000568E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G16" s="4">
@@ -2480,7 +2481,7 @@
         <v>78</v>
       </c>
       <c r="K16">
-        <f>($J16-$J15)/($B16-$B15)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M16">
@@ -2488,7 +2489,7 @@
         <v>78</v>
       </c>
       <c r="N16">
-        <f>($M16-$M15)/($B16-$B15)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2506,11 +2507,11 @@
         <v>78.08</v>
       </c>
       <c r="E17">
-        <f>($D17-$D16)/($B17-$B16)</f>
+        <f t="shared" si="2"/>
         <v>3.0000000000001137E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.03</v>
       </c>
       <c r="G17" s="4">
@@ -2521,7 +2522,7 @@
         <v>78.0625</v>
       </c>
       <c r="K17">
-        <f>($J17-$J16)/($B17-$B16)</f>
+        <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
       <c r="M17">
@@ -2529,7 +2530,7 @@
         <v>78.100000000000009</v>
       </c>
       <c r="N17">
-        <f>($M17-$M16)/($B17-$B16)</f>
+        <f t="shared" si="4"/>
         <v>5.0000000000004263E-2</v>
       </c>
     </row>
@@ -2547,11 +2548,11 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E18">
-        <f>($D18-$D17)/($B18-$B17)</f>
+        <f t="shared" si="2"/>
         <v>9.9999999999980105E-3</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
       <c r="G18" s="4">
@@ -2562,7 +2563,7 @@
         <v>78.125</v>
       </c>
       <c r="K18">
-        <f>($J18-$J17)/($B18-$B17)</f>
+        <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
       <c r="M18">
@@ -2570,7 +2571,7 @@
         <v>78.100000000000009</v>
       </c>
       <c r="N18">
-        <f>($M18-$M17)/($B18-$B17)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2588,11 +2589,11 @@
         <v>78.14</v>
       </c>
       <c r="E19">
-        <f>($D19-$D18)/($B19-$B18)</f>
+        <f t="shared" si="2"/>
         <v>1.3333333333335418E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3000000000000001E-2</v>
       </c>
       <c r="G19" s="4">
@@ -2603,7 +2604,7 @@
         <v>78.125</v>
       </c>
       <c r="K19">
-        <f>($J19-$J18)/($B19-$B18)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M19">
@@ -2611,7 +2612,7 @@
         <v>78.100000000000009</v>
       </c>
       <c r="N19">
-        <f>($M19-$M18)/($B19-$B18)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2629,11 +2630,11 @@
         <v>78.17</v>
       </c>
       <c r="E20">
-        <f>($D20-$D19)/($B20-$B19)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000000378E-2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
       <c r="G20" s="4">
@@ -2644,7 +2645,7 @@
         <v>78.1875</v>
       </c>
       <c r="K20">
-        <f>($J20-$J19)/($B20-$B19)</f>
+        <f t="shared" si="3"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="M20">
@@ -2652,7 +2653,7 @@
         <v>78.2</v>
       </c>
       <c r="N20">
-        <f>($M20-$M19)/($B20-$B19)</f>
+        <f t="shared" si="4"/>
         <v>3.3333333333331439E-2</v>
       </c>
     </row>
@@ -2670,11 +2671,11 @@
         <v>78.209999999999994</v>
       </c>
       <c r="E21">
-        <f>($D21-$D20)/($B21-$B20)</f>
+        <f t="shared" si="2"/>
         <v>1.333333333333068E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3000000000000001E-2</v>
       </c>
       <c r="G21" s="4">
@@ -2685,7 +2686,7 @@
         <v>78.1875</v>
       </c>
       <c r="K21">
-        <f>($J21-$J20)/($B21-$B20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M21">
@@ -2693,7 +2694,7 @@
         <v>78.2</v>
       </c>
       <c r="N21">
-        <f>($M21-$M20)/($B21-$B20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2711,11 +2712,11 @@
         <v>78.23</v>
       </c>
       <c r="E22">
-        <f>($D22-$D21)/($B22-$B21)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000005116E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
       <c r="G22" s="4">
@@ -2726,7 +2727,7 @@
         <v>78.25</v>
       </c>
       <c r="K22">
-        <f>($J22-$J21)/($B22-$B21)</f>
+        <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
       <c r="M22">
@@ -2734,7 +2735,7 @@
         <v>78.2</v>
       </c>
       <c r="N22">
-        <f>($M22-$M21)/($B22-$B21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O22" t="s">
@@ -2755,11 +2756,11 @@
         <v>78.25</v>
       </c>
       <c r="E23">
-        <f>($D23-$D22)/($B23-$B22)</f>
+        <f t="shared" si="2"/>
         <v>1.9999999999996021E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="G23" s="4">
@@ -2770,7 +2771,7 @@
         <v>78.25</v>
       </c>
       <c r="K23">
-        <f>($J23-$J22)/($B23-$B22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M23">
@@ -2778,7 +2779,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N23">
-        <f>($M23-$M22)/($B23-$B22)</f>
+        <f t="shared" si="4"/>
         <v>0.10000000000000853</v>
       </c>
     </row>
@@ -2796,11 +2797,11 @@
         <v>78.27</v>
       </c>
       <c r="E24">
-        <f>($D24-$D23)/($B24-$B23)</f>
+        <f t="shared" si="2"/>
         <v>6.66666666666534E-3</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G24" s="4">
@@ -2811,7 +2812,7 @@
         <v>78.25</v>
       </c>
       <c r="K24">
-        <f>($J24-$J23)/($B24-$B23)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M24">
@@ -2819,7 +2820,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N24">
-        <f>($M24-$M23)/($B24-$B23)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2837,11 +2838,11 @@
         <v>78.28</v>
       </c>
       <c r="E25">
-        <f>($D25-$D24)/($B25-$B24)</f>
+        <f t="shared" si="2"/>
         <v>5.000000000002558E-3</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G25" s="4">
@@ -2852,7 +2853,7 @@
         <v>78.25</v>
       </c>
       <c r="K25">
-        <f>($J25-$J24)/($B25-$B24)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L25" t="s">
@@ -2863,7 +2864,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N25">
-        <f>($M25-$M24)/($B25-$B24)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2881,11 +2882,11 @@
         <v>78.290000000000006</v>
       </c>
       <c r="E26">
-        <f>($D26-$D25)/($B26-$B25)</f>
+        <f t="shared" si="2"/>
         <v>5.000000000002558E-3</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G26" s="4">
@@ -2896,7 +2897,7 @@
         <v>78.3125</v>
       </c>
       <c r="K26">
-        <f>($J26-$J25)/($B26-$B25)</f>
+        <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
       <c r="M26">
@@ -2904,7 +2905,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N26">
-        <f>($M26-$M25)/($B26-$B25)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2922,11 +2923,11 @@
         <v>78.3</v>
       </c>
       <c r="E27">
-        <f>($D27-$D26)/($B27-$B26)</f>
+        <f t="shared" si="2"/>
         <v>9.9999999999909051E-3</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
       <c r="G27" s="4">
@@ -2937,7 +2938,7 @@
         <v>78.3125</v>
       </c>
       <c r="K27">
-        <f>($J27-$J26)/($B27-$B26)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M27">
@@ -2945,7 +2946,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N27">
-        <f>($M27-$M26)/($B27-$B26)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2963,11 +2964,11 @@
         <v>78.3</v>
       </c>
       <c r="E28">
-        <f>($D28-$D27)/($B28-$B27)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G28" s="4">
@@ -2978,7 +2979,7 @@
         <v>78.3125</v>
       </c>
       <c r="K28">
-        <f>($J28-$J27)/($B28-$B27)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M28">
@@ -2986,7 +2987,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N28">
-        <f>($M28-$M27)/($B28-$B27)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3004,11 +3005,11 @@
         <v>78.33</v>
       </c>
       <c r="E29">
-        <f>($D29-$D28)/($B29-$B28)</f>
+        <f t="shared" si="2"/>
         <v>5.0000000000001892E-3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G29" s="4">
@@ -3022,7 +3023,7 @@
         <v>78.3125</v>
       </c>
       <c r="K29">
-        <f>($J29-$J28)/($B29-$B28)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29">
@@ -3030,7 +3031,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N29">
-        <f>($M29-$M28)/($B29-$B28)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3045,11 +3046,11 @@
         <v>78.33</v>
       </c>
       <c r="E30">
-        <f>($D30-$D29)/($B30-$B29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J30">
@@ -3057,7 +3058,7 @@
         <v>78.3125</v>
       </c>
       <c r="K30">
-        <f>($J30-$J29)/($B30-$B29)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M30">
@@ -3065,7 +3066,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N30">
-        <f>($M30-$M29)/($B30-$B29)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3080,11 +3081,11 @@
         <v>78.33</v>
       </c>
       <c r="E31">
-        <f>($D31-$D30)/($B31-$B30)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J31">
@@ -3092,7 +3093,7 @@
         <v>78.3125</v>
       </c>
       <c r="K31">
-        <f>($J31-$J30)/($B31-$B30)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M31">
@@ -3100,7 +3101,7 @@
         <v>78.300000000000011</v>
       </c>
       <c r="N31">
-        <f>($M31-$M30)/($B31-$B30)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>